<commit_message>
Bezeichnung und Kommentare geändert
Bezeichnungen und Kommentare wurden geändert bzw. hinzugefügt
</commit_message>
<xml_diff>
--- a/Dokumentation/Kostenberechnung.xlsx
+++ b/Dokumentation/Kostenberechnung.xlsx
@@ -11,7 +11,7 @@
     <sheet name="Tabelle2" sheetId="2" r:id="rId2"/>
     <sheet name="Tabelle3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="125725"/>
 </workbook>
 </file>
 
@@ -19,6 +19,7 @@
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <authors>
     <author>Marco Wurzenberger</author>
+    <author>admin</author>
   </authors>
   <commentList>
     <comment ref="B2" authorId="0">
@@ -52,6 +53,48 @@
         </r>
       </text>
     </comment>
+    <comment ref="B17" authorId="1">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Die Auslastung beträgt ein Viertel der monatl. Arbeitszeit</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B18" authorId="1">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Projektdauer 3,5 Monate</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B19" authorId="1">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Durch die Neuartigkeit des Projektes akzeptiert die Geschäftsführung ausnahmsweise diesen Preis</t>
+        </r>
+      </text>
+    </comment>
     <comment ref="A21" authorId="0">
       <text>
         <r>
@@ -62,7 +105,8 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>Wir brauchen 3mal so lange wie ein Profi</t>
+          <t>Annahme: 
+Wir brauchen 3mal so lange wie Profis</t>
         </r>
       </text>
     </comment>
@@ -71,31 +115,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
-  <si>
-    <t>Kostenberechnung</t>
-  </si>
-  <si>
-    <t>Gesamt:</t>
-  </si>
-  <si>
-    <t>Lohnnebenkosten:</t>
-  </si>
-  <si>
-    <t>Kosten / Monat:</t>
-  </si>
-  <si>
-    <t>bei 10 Std./Woche:</t>
-  </si>
-  <si>
-    <t>mal 3,5 (Monate):</t>
-  </si>
-  <si>
-    <t>Ges. Personalkosten:</t>
-  </si>
-  <si>
-    <t>Durch 3:</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
   <si>
     <t>Personen:</t>
   </si>
@@ -103,22 +123,49 @@
     <t>Stunden Gesamt:</t>
   </si>
   <si>
-    <t>Lohn bei Angestellten:</t>
-  </si>
-  <si>
-    <t>+ Urlaubsgeld:</t>
-  </si>
-  <si>
-    <t>+ Weihnachtsgeld:</t>
-  </si>
-  <si>
-    <t>Stunden  / Woche:</t>
-  </si>
-  <si>
     <t>Projektdauer bzw. Wochen:</t>
   </si>
   <si>
-    <t>Stunden aller Personen:</t>
+    <t>Stunden pro Woche:</t>
+  </si>
+  <si>
+    <t>Mannstunden gesamt:</t>
+  </si>
+  <si>
+    <t>Bruttogehalt pro Mitarbeiter</t>
+  </si>
+  <si>
+    <t>+ aliquot Weihnachtsgeld:</t>
+  </si>
+  <si>
+    <t>+ aliquot Urlaubsgeld:</t>
+  </si>
+  <si>
+    <t>Durchschn. Monatsbezug:</t>
+  </si>
+  <si>
+    <t>Lohnnebenkosten 30% :</t>
+  </si>
+  <si>
+    <t>Kosten pro Monat und Mitarbeiter:</t>
+  </si>
+  <si>
+    <t>bei 10 Stunden pro Woche:</t>
+  </si>
+  <si>
+    <t>Istkosten eines Mitarbeiters:</t>
+  </si>
+  <si>
+    <t>Kostenberechnung Reisebüro Graf</t>
+  </si>
+  <si>
+    <t>Ist-Personalkosten IT-Fox (Gesamt):</t>
+  </si>
+  <si>
+    <t>Realistische Personalkosten lt. GF</t>
+  </si>
+  <si>
+    <t>Preisuntergrenze für unser Angebot</t>
   </si>
 </sst>
 </file>
@@ -572,15 +619,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C21"/>
+  <dimension ref="A1:D21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+      <selection activeCell="F19" sqref="F19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="30.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="37.7109375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="13.28515625" style="1" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="2.28515625" customWidth="1"/>
     <col min="4" max="4" width="20.7109375" bestFit="1" customWidth="1"/>
@@ -588,13 +635,13 @@
   <sheetData>
     <row r="1" spans="1:2" ht="24.75" customHeight="1">
       <c r="A1" s="14" t="s">
-        <v>0</v>
+        <v>13</v>
       </c>
       <c r="B1" s="14"/>
     </row>
     <row r="2" spans="1:2" ht="16.5">
       <c r="A2" s="4" t="s">
-        <v>13</v>
+        <v>3</v>
       </c>
       <c r="B2" s="3">
         <v>10</v>
@@ -602,7 +649,7 @@
     </row>
     <row r="3" spans="1:2" ht="16.5">
       <c r="A3" s="4" t="s">
-        <v>14</v>
+        <v>2</v>
       </c>
       <c r="B3" s="3">
         <v>14</v>
@@ -610,7 +657,7 @@
     </row>
     <row r="4" spans="1:2" ht="16.5">
       <c r="A4" s="5" t="s">
-        <v>9</v>
+        <v>1</v>
       </c>
       <c r="B4" s="6">
         <f>B2*B3</f>
@@ -623,7 +670,7 @@
     </row>
     <row r="6" spans="1:2" ht="16.5">
       <c r="A6" s="4" t="s">
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="B6" s="7">
         <v>9</v>
@@ -631,7 +678,7 @@
     </row>
     <row r="7" spans="1:2" ht="16.5">
       <c r="A7" s="5" t="s">
-        <v>15</v>
+        <v>4</v>
       </c>
       <c r="B7" s="6">
         <f>B4*B6</f>
@@ -644,7 +691,7 @@
     </row>
     <row r="9" spans="1:2" ht="16.5">
       <c r="A9" s="4" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="B9" s="13">
         <v>2400</v>
@@ -652,7 +699,7 @@
     </row>
     <row r="10" spans="1:2" ht="16.5">
       <c r="A10" s="8" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="B10" s="11">
         <f>B9/12</f>
@@ -661,7 +708,7 @@
     </row>
     <row r="11" spans="1:2" ht="16.5">
       <c r="A11" s="8" t="s">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="B11" s="11">
         <f>B9/12</f>
@@ -670,7 +717,7 @@
     </row>
     <row r="12" spans="1:2" ht="16.5">
       <c r="A12" s="5" t="s">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="B12" s="12">
         <f>SUM(B9:B11)</f>
@@ -683,7 +730,7 @@
     </row>
     <row r="14" spans="1:2" ht="16.5">
       <c r="A14" s="4" t="s">
-        <v>2</v>
+        <v>9</v>
       </c>
       <c r="B14" s="11">
         <v>840</v>
@@ -691,7 +738,7 @@
     </row>
     <row r="15" spans="1:2" ht="16.5">
       <c r="A15" s="5" t="s">
-        <v>3</v>
+        <v>10</v>
       </c>
       <c r="B15" s="12">
         <f>B12+B14</f>
@@ -702,46 +749,49 @@
       <c r="A16" s="4"/>
       <c r="B16" s="3"/>
     </row>
-    <row r="17" spans="1:3" ht="16.5">
+    <row r="17" spans="1:4" ht="16.5">
       <c r="A17" s="4" t="s">
-        <v>4</v>
+        <v>11</v>
       </c>
       <c r="B17" s="11">
         <f>B15/4</f>
         <v>910</v>
       </c>
     </row>
-    <row r="18" spans="1:3" ht="16.5">
+    <row r="18" spans="1:4" ht="16.5">
       <c r="A18" s="4" t="s">
-        <v>5</v>
+        <v>12</v>
       </c>
       <c r="B18" s="11">
         <f>B17*3.5</f>
         <v>3185</v>
       </c>
     </row>
-    <row r="19" spans="1:3" ht="16.5">
+    <row r="19" spans="1:4" ht="16.5">
       <c r="A19" s="5" t="s">
-        <v>6</v>
+        <v>14</v>
       </c>
       <c r="B19" s="12">
         <f>B18*B6</f>
         <v>28665</v>
       </c>
     </row>
-    <row r="20" spans="1:3" ht="16.5">
+    <row r="20" spans="1:4" ht="16.5">
       <c r="A20" s="4"/>
       <c r="B20" s="3"/>
     </row>
-    <row r="21" spans="1:3" ht="17.25" thickBot="1">
+    <row r="21" spans="1:4" ht="17.25" thickBot="1">
       <c r="A21" s="9" t="s">
-        <v>7</v>
+        <v>15</v>
       </c>
       <c r="B21" s="10">
         <f>B19/3</f>
         <v>9555</v>
       </c>
       <c r="C21" s="2"/>
+      <c r="D21" s="4" t="s">
+        <v>16</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>